<commit_message>
Tabelle per confronto complete
</commit_message>
<xml_diff>
--- a/Progetto 1/Grafici per confronto.xlsx
+++ b/Progetto 1/Grafici per confronto.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
   <si>
     <t>GT01R</t>
   </si>
@@ -463,11 +463,15 @@
       <c r="C4" s="1">
         <v>9.3314999999999995E-2</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1">
+        <v>0.21237</v>
+      </c>
       <c r="E4" s="1">
         <v>0.94505899999999998</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <v>1.160633</v>
+      </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="1" t="s">
@@ -476,11 +480,15 @@
       <c r="C5" s="1">
         <v>0.29393000000000002</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>0.48635</v>
+      </c>
       <c r="E5" s="1">
         <v>1.574614</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>0.799041</v>
+      </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="1" t="s">
@@ -489,11 +497,15 @@
       <c r="C6" s="1">
         <v>0.71318000000000004</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>0.93281000000000003</v>
+      </c>
       <c r="E6" s="1">
         <v>11.586387999999999</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>5.7427640000000002</v>
+      </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
@@ -502,11 +514,15 @@
       <c r="C7" s="3">
         <v>26.277999999999999</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>44.357999999999997</v>
+      </c>
       <c r="E7" s="1">
         <v>32.805546999999997</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>31.489097999999998</v>
+      </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
@@ -515,11 +531,15 @@
       <c r="C8" s="4">
         <v>1.1106</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>1.2057</v>
+      </c>
       <c r="E8" s="1">
         <v>4.6433</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>4.0573240000000004</v>
+      </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="1" t="s">
@@ -528,11 +548,15 @@
       <c r="C9" s="4">
         <v>1.6984999999999999</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>1.9883</v>
+      </c>
       <c r="E9" s="1">
         <v>1.9132709999999999</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>1.736672</v>
+      </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="1" t="s">
@@ -541,11 +565,15 @@
       <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="1" t="s">
@@ -554,11 +582,15 @@
       <c r="C11" s="4">
         <v>5.2464000000000004</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>8.4802999999999997</v>
+      </c>
       <c r="E11" s="1">
         <v>6.4567160000000001</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>6.3065340000000001</v>
+      </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="1"/>
@@ -596,11 +628,15 @@
       <c r="C15" s="2">
         <v>3.8098999999999998E-15</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1">
+        <v>4.5755000000000003E-15</v>
+      </c>
       <c r="E15" s="2">
         <v>8.2008600000000001E-13</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1">
+        <v>5.8967999999999997E-13</v>
+      </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="1" t="s">
@@ -609,11 +645,15 @@
       <c r="C16" s="2">
         <v>7.1178999999999998E-12</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1">
+        <v>6.9070000000000004E-12</v>
+      </c>
       <c r="E16" s="1">
         <v>5.3789999999999996E-12</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1">
+        <v>1.7543000000000001E-11</v>
+      </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="1" t="s">
@@ -622,11 +662,15 @@
       <c r="C17" s="2">
         <v>9.3889999999999993E-16</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="2">
+        <v>9.2759999999999993E-16</v>
+      </c>
       <c r="E17" s="1">
         <v>7.8831000000000006E-15</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1">
+        <v>9.5781E-15</v>
+      </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="1" t="s">
@@ -635,11 +679,15 @@
       <c r="C18" s="2">
         <v>4.5005999999999999E-11</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1">
+        <v>7.0047000000000006E-11</v>
+      </c>
       <c r="E18" s="1">
         <v>3.6637000000000002E-11</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1">
+        <v>2.7592999999999998E-11</v>
+      </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="1" t="s">
@@ -648,11 +696,15 @@
       <c r="C19" s="2">
         <v>3.3311000000000002E-14</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1">
+        <v>3.3264000000000001E-14</v>
+      </c>
       <c r="E19" s="1">
         <v>3.7516000000000001E-14</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1">
+        <v>4.0285000000000002E-14</v>
+      </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="1" t="s">
@@ -661,11 +713,15 @@
       <c r="C20" s="2">
         <v>1.1209999999999999E-5</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="2">
+        <v>1.1209999999999999E-5</v>
+      </c>
       <c r="E20" s="2">
         <v>5.959E-6</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1">
+        <v>6.0720999999999999E-6</v>
+      </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" s="1" t="s">
@@ -674,11 +730,15 @@
       <c r="C21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="1" t="s">
@@ -687,11 +747,15 @@
       <c r="C22" s="1">
         <v>3.575E-12</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1">
+        <v>2.9140999999999999E-12</v>
+      </c>
       <c r="E22" s="1">
         <v>4.8900000000000004E-12</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1">
+        <v>4.9376999999999999E-12</v>
+      </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="1"/>
@@ -729,11 +793,15 @@
       <c r="C26" s="1">
         <v>27</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1">
+        <v>18</v>
+      </c>
       <c r="E26" s="5">
         <v>49</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="1" t="s">
@@ -742,11 +810,15 @@
       <c r="C27" s="1">
         <v>28</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1">
+        <v>25</v>
+      </c>
       <c r="E27" s="1">
         <v>75</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="1">
+        <v>18</v>
+      </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="1" t="s">
@@ -755,11 +827,15 @@
       <c r="C28" s="1">
         <v>268</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1">
+        <v>214</v>
+      </c>
       <c r="E28" s="1">
         <v>333</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="1">
+        <v>248</v>
+      </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="1" t="s">
@@ -768,11 +844,15 @@
       <c r="C29" s="5">
         <v>7089</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="1">
+        <v>6900</v>
+      </c>
       <c r="E29" s="1">
         <v>2551</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1">
+        <v>2302</v>
+      </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="1" t="s">
@@ -781,11 +861,15 @@
       <c r="C30" s="5">
         <v>430</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1">
+        <v>108</v>
+      </c>
       <c r="E30" s="1">
         <v>595</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="1">
+        <v>547</v>
+      </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="1" t="s">
@@ -794,11 +878,15 @@
       <c r="C31" s="5">
         <v>554</v>
       </c>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1">
+        <v>314</v>
+      </c>
       <c r="E31" s="1">
         <v>313</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1">
+        <v>348</v>
+      </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="1" t="s">
@@ -807,11 +895,15 @@
       <c r="C32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="1" t="s">
@@ -820,11 +912,15 @@
       <c r="C33" s="5">
         <v>2399</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="1">
+        <v>2304</v>
+      </c>
       <c r="E33" s="1">
         <v>2047</v>
       </c>
-      <c r="F33" s="1"/>
+      <c r="F33" s="1">
+        <v>2472</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>